<commit_message>
returned old version of Data.xlsx which was accidentally deleted
</commit_message>
<xml_diff>
--- a/docs/examples and guides/Example1/Data.xlsx
+++ b/docs/examples and guides/Example1/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc\Atmonia Dropbox\Marc Francis Hidalgo\Scripts\How to DoE and ML\ML\docs\examples and guides\input data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jlrglobal-my.sharepoint.com/personal/mhidalgo_jaguarlandrover_com/Documents/Projects/ML/docs/examples and guides/auto_mlr_notebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70CEEA9-DA9F-4A04-86DE-EBCBFB3C4018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{C70CEEA9-DA9F-4A04-86DE-EBCBFB3C4018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF80691D-93F4-42B6-942D-FEAF15D24473}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{C1646789-F2F7-4596-96D5-A1743CEE8B52}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{C1646789-F2F7-4596-96D5-A1743CEE8B52}"/>
   </bookViews>
   <sheets>
     <sheet name="Train Data" sheetId="4" r:id="rId1"/>
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>Features</t>
   </si>
@@ -222,10 +222,13 @@
     <t>Numerical</t>
   </si>
   <si>
-    <t>version</t>
-  </si>
-  <si>
     <t>-2,-1,-0.5,0,0.5,1,2</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>Linear</t>
   </si>
 </sst>
 </file>
@@ -690,9 +693,9 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -712,7 +715,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -732,7 +735,7 @@
         <v>72.041289257868158</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -752,7 +755,7 @@
         <v>85.186684022091868</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -772,7 +775,7 @@
         <v>89.828855429747492</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -792,7 +795,7 @@
         <v>59.174622450856383</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>6</v>
       </c>
@@ -812,7 +815,7 @@
         <v>84.951190961672879</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>7</v>
       </c>
@@ -832,7 +835,7 @@
         <v>30.733031121982521</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>8</v>
       </c>
@@ -852,7 +855,7 @@
         <v>84.945758440531378</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>9</v>
       </c>
@@ -872,7 +875,7 @@
         <v>69.421891154692503</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>10</v>
       </c>
@@ -892,7 +895,7 @@
         <v>8.8965527938430003E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>12</v>
       </c>
@@ -912,7 +915,7 @@
         <v>11.601307424285451</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>13</v>
       </c>
@@ -932,7 +935,7 @@
         <v>3.4966099123584069</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>14</v>
       </c>
@@ -952,7 +955,7 @@
         <v>17.198715402852347</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>15</v>
       </c>
@@ -972,7 +975,7 @@
         <v>14.892530662050966</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>16</v>
       </c>
@@ -992,7 +995,7 @@
         <v>8.9214094531340604E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>17</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>15.862730271587914</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>5</v>
       </c>
@@ -1032,7 +1035,7 @@
         <v>81.773996381057302</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>11</v>
       </c>
@@ -1052,7 +1055,7 @@
         <v>21.636350153652174</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -1087,9 +1090,9 @@
       <selection activeCell="A2" sqref="A2:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1109,7 +1112,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>5</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>81.773996381057302</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>11</v>
       </c>
@@ -1149,7 +1152,7 @@
         <v>21.636350153652174</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>18</v>
       </c>
@@ -1184,17 +1187,17 @@
       <selection activeCell="C3" sqref="C3:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="40.90625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="8.7265625" style="1"/>
-    <col min="6" max="6" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.7109375" style="1"/>
+    <col min="2" max="2" width="40.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.7109375" style="1"/>
+    <col min="6" max="6" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1214,7 +1217,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1234,7 +1237,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1254,7 +1257,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1292,18 +1295,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A8F6C1-4570-407C-96BE-50A819E04C7D}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.7265625" style="1"/>
+    <col min="3" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1311,20 +1314,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1337,21 +1340,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996A7378-54BB-494D-84D1-CDC0B6ABA572}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1">
-        <v>0.2</v>
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{C4F75C21-3D0E-4D31-9DA3-D6EE1298B439}">
+      <formula1>"Linear, 2FI, Quadratic"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>